<commit_message>
Concluida criacao de campos da tabela produto_mobly
</commit_message>
<xml_diff>
--- a/base/Template_Mobly.xlsx
+++ b/base/Template_Mobly.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6581" uniqueCount="5540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6612" uniqueCount="5568">
   <si>
     <t>Campo</t>
   </si>
@@ -16645,6 +16645,90 @@
   </si>
   <si>
     <t>PRO_DESCRICAO</t>
+  </si>
+  <si>
+    <t>MOB_COLOR</t>
+  </si>
+  <si>
+    <t>MOB_COLOR_FAMILY</t>
+  </si>
+  <si>
+    <t>MOB_MATERIAL</t>
+  </si>
+  <si>
+    <t>MOB_MATERIAL_FAMILY</t>
+  </si>
+  <si>
+    <t>MOB_PRODUCT_WARRANTY</t>
+  </si>
+  <si>
+    <t>MOB_WEIGHT_CAPACITY</t>
+  </si>
+  <si>
+    <t>MOB_DIMENSIONS</t>
+  </si>
+  <si>
+    <t>MOB_WATT</t>
+  </si>
+  <si>
+    <t>MOB_INDICATE_AGE</t>
+  </si>
+  <si>
+    <t>MOB_FOR_MATTRESS_TYPE</t>
+  </si>
+  <si>
+    <t>MOB_NUMBER_OF_PIECES</t>
+  </si>
+  <si>
+    <t>MOB_SEAT_GROUND_HEIGHT</t>
+  </si>
+  <si>
+    <t>MOB_RECOMMENDED_WEIGHT_CH</t>
+  </si>
+  <si>
+    <t>MOB_PAINTING_FINISHING</t>
+  </si>
+  <si>
+    <t>MOB_COATING</t>
+  </si>
+  <si>
+    <t>MOB_TYPE</t>
+  </si>
+  <si>
+    <t>MOB_MATERIAL_TABLE_TOP</t>
+  </si>
+  <si>
+    <t>MOB_FORMAT_GI</t>
+  </si>
+  <si>
+    <t>MOB_DECORATIVE</t>
+  </si>
+  <si>
+    <t>MOB_TYPE_OF_FOOT_GI</t>
+  </si>
+  <si>
+    <t>MOB_NUMBER_OF_DOORS</t>
+  </si>
+  <si>
+    <t>MOB_NUMBER_OF_DRAWERS</t>
+  </si>
+  <si>
+    <t>MOB_NUMBER_OF_SHELVES</t>
+  </si>
+  <si>
+    <t>MOB_LAMP_NUMBER</t>
+  </si>
+  <si>
+    <t>MOB_GLOBAL_CAPACITY</t>
+  </si>
+  <si>
+    <t>MOB_SOCKET_TYPE</t>
+  </si>
+  <si>
+    <t>MOB_VOLTAGE_HW</t>
+  </si>
+  <si>
+    <t>MOB_ASSEMBLY_REQUIRED</t>
   </si>
 </sst>
 </file>
@@ -16803,7 +16887,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -16836,9 +16920,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -17171,8 +17252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17180,7 +17261,7 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
     <col min="5" max="5" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" bestFit="1" customWidth="1"/>
@@ -17188,22 +17269,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>5520</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>5537</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -17214,10 +17295,10 @@
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>5521</v>
       </c>
-      <c r="D2" s="20" t="str">
+      <c r="D2" s="19" t="str">
         <f>CONCATENATE(C2, " AS `", B2, "`,")</f>
         <v>PRO_NOME AS `Name`,</v>
       </c>
@@ -17236,10 +17317,10 @@
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>5527</v>
       </c>
-      <c r="D3" s="20" t="str">
+      <c r="D3" s="19" t="str">
         <f t="shared" ref="D3:D66" si="0">CONCATENATE(C3, " AS `", B3, "`,")</f>
         <v>FOR_NOME AS `Brand`,</v>
       </c>
@@ -17258,10 +17339,10 @@
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>5528</v>
       </c>
-      <c r="D4" s="20" t="str">
+      <c r="D4" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_REF AS `Model`,</v>
       </c>
@@ -17280,10 +17361,10 @@
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>5522</v>
       </c>
-      <c r="D5" s="20" t="str">
+      <c r="D5" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_GTIN AS `ProductId`,</v>
       </c>
@@ -17300,10 +17381,10 @@
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>5528</v>
       </c>
-      <c r="D6" s="20" t="str">
+      <c r="D6" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_REF AS `SellerSKU`,</v>
       </c>
@@ -17322,10 +17403,10 @@
       <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>5528</v>
       </c>
-      <c r="D7" s="20" t="str">
+      <c r="D7" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_REF AS `ParentSKU`,</v>
       </c>
@@ -17344,10 +17425,10 @@
       <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>5523</v>
       </c>
-      <c r="D8" s="20" t="str">
+      <c r="D8" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_ESTOQUE AS `Quantity`,</v>
       </c>
@@ -17366,10 +17447,10 @@
       <c r="B9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>5524</v>
       </c>
-      <c r="D9" s="20" t="str">
+      <c r="D9" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_ALTURA AS `BoxHeight`,</v>
       </c>
@@ -17390,10 +17471,10 @@
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>5525</v>
       </c>
-      <c r="D10" s="20" t="str">
+      <c r="D10" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_LARGURA AS `BoxWidth`,</v>
       </c>
@@ -17414,10 +17495,10 @@
       <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>5526</v>
       </c>
-      <c r="D11" s="20" t="str">
+      <c r="D11" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_COMPRIMENTO AS `BoxLength`,</v>
       </c>
@@ -17438,10 +17519,10 @@
       <c r="B12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>5530</v>
       </c>
-      <c r="D12" s="20" t="str">
+      <c r="D12" s="19" t="str">
         <f t="shared" si="0"/>
         <v>ROUND(PRO_PESO / 1000, 2) AS `BoxWeight`,</v>
       </c>
@@ -17462,10 +17543,10 @@
       <c r="B13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>5529</v>
       </c>
-      <c r="D13" s="20" t="str">
+      <c r="D13" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_DIAS_PRAZO AS `SupplierDeliveryTime`,</v>
       </c>
@@ -17484,10 +17565,10 @@
       <c r="B14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>5524</v>
       </c>
-      <c r="D14" s="20" t="str">
+      <c r="D14" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_ALTURA AS `ProductHeight`,</v>
       </c>
@@ -17508,10 +17589,10 @@
       <c r="B15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>5525</v>
       </c>
-      <c r="D15" s="20" t="str">
+      <c r="D15" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_LARGURA AS `ProductWidth`,</v>
       </c>
@@ -17532,10 +17613,10 @@
       <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>5526</v>
       </c>
-      <c r="D16" s="20" t="str">
+      <c r="D16" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_COMPRIMENTO AS `ProductLength`,</v>
       </c>
@@ -17556,10 +17637,10 @@
       <c r="B17" s="8" t="s">
         <v>5512</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>5530</v>
       </c>
-      <c r="D17" s="20" t="str">
+      <c r="D17" s="19" t="str">
         <f t="shared" si="0"/>
         <v>ROUND(PRO_PESO / 1000, 2) AS `ProductWeight`,</v>
       </c>
@@ -17580,10 +17661,10 @@
       <c r="B18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>5531</v>
       </c>
-      <c r="D18" s="20" t="str">
+      <c r="D18" s="19" t="str">
         <f t="shared" si="0"/>
         <v>CONCAT(PRO_ALTURA,'x',PRO_LARGURA,'x',PRO_COMPRIMENTO,'cm') AS `SizeDescription`,</v>
       </c>
@@ -17604,10 +17685,12 @@
       <c r="B19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20" t="str">
+      <c r="C19" s="19" t="s">
+        <v>5540</v>
+      </c>
+      <c r="D19" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Color`,</v>
+        <v>MOB_COLOR AS `Color`,</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>5482</v>
@@ -17626,10 +17709,12 @@
       <c r="B20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20" t="str">
+      <c r="C20" s="19" t="s">
+        <v>5541</v>
+      </c>
+      <c r="D20" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `ColorFamily`,</v>
+        <v>MOB_COLOR_FAMILY AS `ColorFamily`,</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>5485</v>
@@ -17648,10 +17733,12 @@
       <c r="B21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20" t="str">
+      <c r="C21" s="19" t="s">
+        <v>5542</v>
+      </c>
+      <c r="D21" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Material`,</v>
+        <v>MOB_MATERIAL AS `Material`,</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>5484</v>
@@ -17670,10 +17757,12 @@
       <c r="B22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20" t="str">
+      <c r="C22" s="19" t="s">
+        <v>5543</v>
+      </c>
+      <c r="D22" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `MaterialFamily`,</v>
+        <v>MOB_MATERIAL_FAMILY AS `MaterialFamily`,</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>5486</v>
@@ -17692,10 +17781,10 @@
       <c r="B23" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>5532</v>
       </c>
-      <c r="D23" s="20" t="str">
+      <c r="D23" s="19" t="str">
         <f t="shared" si="0"/>
         <v>ROUND(PRO_VALOR,2) AS `Price`,</v>
       </c>
@@ -17714,10 +17803,10 @@
       <c r="B24" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="19" t="s">
         <v>5533</v>
       </c>
-      <c r="D24" s="20" t="str">
+      <c r="D24" s="19" t="str">
         <f t="shared" si="0"/>
         <v>ROUND(PRO_PROMOCAO,2) AS `SalePrice`,</v>
       </c>
@@ -17736,10 +17825,10 @@
       <c r="B25" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="19" t="s">
         <v>5534</v>
       </c>
-      <c r="D25" s="20" t="str">
+      <c r="D25" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_PROMO_INI AS `SaleStartDate`,</v>
       </c>
@@ -17758,10 +17847,10 @@
       <c r="B26" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>5535</v>
       </c>
-      <c r="D26" s="20" t="str">
+      <c r="D26" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_PROMO_FIM AS `SaleEndDate`,</v>
       </c>
@@ -17780,11 +17869,11 @@
       <c r="B27" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="23" t="str">
+      <c r="C27" s="22" t="str">
         <f>"''"</f>
         <v>''</v>
       </c>
-      <c r="D27" s="20" t="str">
+      <c r="D27" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'' AS `PrimaryCategory`,</v>
       </c>
@@ -17801,11 +17890,11 @@
       <c r="B28" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="23" t="str">
+      <c r="C28" s="22" t="str">
         <f t="shared" ref="C28:C35" si="1">"''"</f>
         <v>''</v>
       </c>
-      <c r="D28" s="20" t="str">
+      <c r="D28" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'' AS `Categories`,</v>
       </c>
@@ -17822,11 +17911,11 @@
       <c r="B29" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="23" t="str">
+      <c r="C29" s="22" t="str">
         <f t="shared" si="1"/>
         <v>''</v>
       </c>
-      <c r="D29" s="20" t="str">
+      <c r="D29" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'' AS `AnchorCategory`,</v>
       </c>
@@ -17843,11 +17932,11 @@
       <c r="B30" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="23" t="str">
+      <c r="C30" s="22" t="str">
         <f t="shared" si="1"/>
         <v>''</v>
       </c>
-      <c r="D30" s="20" t="str">
+      <c r="D30" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'' AS `RepProductCategory`,</v>
       </c>
@@ -17864,11 +17953,11 @@
       <c r="B31" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="23" t="str">
+      <c r="C31" s="22" t="str">
         <f t="shared" si="1"/>
         <v>''</v>
       </c>
-      <c r="D31" s="20" t="str">
+      <c r="D31" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'' AS `RepCategoryOtb`,</v>
       </c>
@@ -17885,11 +17974,11 @@
       <c r="B32" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="23" t="str">
+      <c r="C32" s="22" t="str">
         <f t="shared" si="1"/>
         <v>''</v>
       </c>
-      <c r="D32" s="20" t="str">
+      <c r="D32" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'' AS `RepProductDepartment`,</v>
       </c>
@@ -17906,11 +17995,11 @@
       <c r="B33" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="23" t="str">
+      <c r="C33" s="22" t="str">
         <f t="shared" si="1"/>
         <v>''</v>
       </c>
-      <c r="D33" s="20" t="str">
+      <c r="D33" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'' AS `Manager`,</v>
       </c>
@@ -17927,11 +18016,11 @@
       <c r="B34" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="23" t="str">
+      <c r="C34" s="22" t="str">
         <f t="shared" si="1"/>
         <v>''</v>
       </c>
-      <c r="D34" s="20" t="str">
+      <c r="D34" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'' AS `GroupCategoryOtb`,</v>
       </c>
@@ -17948,11 +18037,11 @@
       <c r="B35" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="23" t="str">
+      <c r="C35" s="22" t="str">
         <f t="shared" si="1"/>
         <v>''</v>
       </c>
-      <c r="D35" s="20" t="str">
+      <c r="D35" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'' AS `RepProductSubcategory`,</v>
       </c>
@@ -17969,10 +18058,12 @@
       <c r="B36" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20" t="str">
+      <c r="C36" s="19" t="s">
+        <v>5544</v>
+      </c>
+      <c r="D36" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `ProductWarranty`,</v>
+        <v>MOB_PRODUCT_WARRANTY AS `ProductWarranty`,</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>76</v>
@@ -17991,10 +18082,12 @@
       <c r="B37" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20" t="str">
+      <c r="C37" s="19" t="s">
+        <v>5540</v>
+      </c>
+      <c r="D37" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `ColorSimple`,</v>
+        <v>MOB_COLOR AS `ColorSimple`,</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>79</v>
@@ -18011,10 +18104,12 @@
       <c r="B38" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20" t="str">
+      <c r="C38" s="19" t="s">
+        <v>5541</v>
+      </c>
+      <c r="D38" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `ColorSupplier`,</v>
+        <v>MOB_COLOR_FAMILY AS `ColorSupplier`,</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>80</v>
@@ -18031,10 +18126,12 @@
       <c r="B39" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20" t="str">
+      <c r="C39" s="19" t="s">
+        <v>5521</v>
+      </c>
+      <c r="D39" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `SupplierSimpleName`,</v>
+        <v>PRO_NOME AS `SupplierSimpleName`,</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>86</v>
@@ -18049,11 +18146,11 @@
       <c r="B40" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="20" t="str">
+      <c r="C40" s="19" t="str">
         <f>"'Único'"</f>
         <v>'Único'</v>
       </c>
-      <c r="D40" s="20" t="str">
+      <c r="D40" s="19" t="str">
         <f t="shared" si="0"/>
         <v>'Único' AS `Variation`,</v>
       </c>
@@ -18072,10 +18169,10 @@
       <c r="B41" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="19" t="s">
         <v>5536</v>
       </c>
-      <c r="D41" s="20" t="str">
+      <c r="D41" s="19" t="str">
         <f t="shared" si="0"/>
         <v>IF(PRO_SOB_ENCOMENDA=1, 'Importado', 'Nacional') AS `OriginCountry`,</v>
       </c>
@@ -18094,10 +18191,10 @@
       <c r="B42" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="19" t="s">
         <v>5538</v>
       </c>
-      <c r="D42" s="20" t="str">
+      <c r="D42" s="19" t="str">
         <f t="shared" si="0"/>
         <v>(SELECT CON_UF_LOJA FROM config LIMIT 0,1) AS `OriginState`,</v>
       </c>
@@ -18116,10 +18213,10 @@
       <c r="B43" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="19" t="s">
         <v>5539</v>
       </c>
-      <c r="D43" s="20" t="str">
+      <c r="D43" s="19" t="str">
         <f t="shared" si="0"/>
         <v>PRO_DESCRICAO AS `Description`,</v>
       </c>
@@ -18136,10 +18233,13 @@
       <c r="B44" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20" t="str">
+      <c r="C44" s="19" t="str">
+        <f>"''"</f>
+        <v>''</v>
+      </c>
+      <c r="D44" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `ProductContents`,</v>
+        <v>'' AS `ProductContents`,</v>
       </c>
       <c r="E44" s="15" t="s">
         <v>100</v>
@@ -18154,10 +18254,13 @@
       <c r="B45" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="20" t="str">
+      <c r="C45" s="19" t="str">
+        <f>"''"</f>
+        <v>''</v>
+      </c>
+      <c r="D45" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `ProductInstructions`,</v>
+        <v>'' AS `ProductInstructions`,</v>
       </c>
       <c r="E45" s="17" t="s">
         <v>101</v>
@@ -18172,10 +18275,13 @@
       <c r="B46" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="20" t="str">
+      <c r="C46" s="19" t="str">
+        <f t="shared" ref="C46:C50" si="2">"''"</f>
+        <v>''</v>
+      </c>
+      <c r="D46" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `MainImage`,</v>
+        <v>'' AS `MainImage`,</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>5515</v>
@@ -18190,10 +18296,13 @@
       <c r="B47" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="20" t="str">
+      <c r="C47" s="19" t="str">
+        <f t="shared" si="2"/>
+        <v>''</v>
+      </c>
+      <c r="D47" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Image2`,</v>
+        <v>'' AS `Image2`,</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>5516</v>
@@ -18208,10 +18317,13 @@
       <c r="B48" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="20" t="str">
+      <c r="C48" s="19" t="str">
+        <f t="shared" si="2"/>
+        <v>''</v>
+      </c>
+      <c r="D48" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Image3`,</v>
+        <v>'' AS `Image3`,</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>5517</v>
@@ -18226,10 +18338,13 @@
       <c r="B49" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="20" t="str">
+      <c r="C49" s="19" t="str">
+        <f t="shared" si="2"/>
+        <v>''</v>
+      </c>
+      <c r="D49" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Image4`,</v>
+        <v>'' AS `Image4`,</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>5518</v>
@@ -18244,10 +18359,13 @@
       <c r="B50" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="20" t="str">
+      <c r="C50" s="19" t="str">
+        <f t="shared" si="2"/>
+        <v>''</v>
+      </c>
+      <c r="D50" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Image5`,</v>
+        <v>'' AS `Image5`,</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>5519</v>
@@ -18262,10 +18380,12 @@
       <c r="B51" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="20" t="str">
+      <c r="C51" s="21" t="s">
+        <v>5545</v>
+      </c>
+      <c r="D51" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `WeightCapacity`,</v>
+        <v>MOB_WEIGHT_CAPACITY AS `WeightCapacity`,</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>5493</v>
@@ -18279,13 +18399,15 @@
       <c r="A52" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="20" t="str">
+      <c r="C52" s="21" t="s">
+        <v>5546</v>
+      </c>
+      <c r="D52" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Dimensions`,</v>
+        <v>MOB_DIMENSIONS AS `Dimensions`,</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>5511</v>
@@ -18299,13 +18421,15 @@
       <c r="A53" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="20" t="str">
+      <c r="C53" s="21" t="s">
+        <v>5547</v>
+      </c>
+      <c r="D53" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Watt`,</v>
+        <v>MOB_WATT AS `Watt`,</v>
       </c>
       <c r="E53" s="14" t="s">
         <v>5510</v>
@@ -18319,13 +18443,15 @@
       <c r="A54" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="B54" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="20" t="str">
+      <c r="C54" s="21" t="s">
+        <v>5548</v>
+      </c>
+      <c r="D54" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `IndicatedAge`,</v>
+        <v>MOB_INDICATE_AGE AS `IndicatedAge`,</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>5509</v>
@@ -18339,13 +18465,15 @@
       <c r="A55" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="B55" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C55" s="22"/>
-      <c r="D55" s="20" t="str">
+      <c r="C55" s="21" t="s">
+        <v>5549</v>
+      </c>
+      <c r="D55" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `ForMattressType`,</v>
+        <v>MOB_FOR_MATTRESS_TYPE AS `ForMattressType`,</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>5508</v>
@@ -18359,13 +18487,15 @@
       <c r="A56" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="B56" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="22"/>
-      <c r="D56" s="20" t="str">
+      <c r="C56" s="21" t="s">
+        <v>5550</v>
+      </c>
+      <c r="D56" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `NumberOfPieces`,</v>
+        <v>MOB_NUMBER_OF_PIECES AS `NumberOfPieces`,</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>5507</v>
@@ -18379,13 +18509,15 @@
       <c r="A57" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="18" t="s">
         <v>5487</v>
       </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="20" t="str">
+      <c r="C57" s="21" t="s">
+        <v>5551</v>
+      </c>
+      <c r="D57" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `SeatGroundHeight`,</v>
+        <v>MOB_SEAT_GROUND_HEIGHT AS `SeatGroundHeight`,</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>5506</v>
@@ -18401,13 +18533,15 @@
       <c r="A58" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="18" t="s">
         <v>5488</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="20" t="str">
+      <c r="C58" s="21" t="s">
+        <v>5552</v>
+      </c>
+      <c r="D58" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `RecommendedWeightCh`,</v>
+        <v>MOB_RECOMMENDED_WEIGHT_CH AS `RecommendedWeightCh`,</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>5505</v>
@@ -18423,13 +18557,15 @@
       <c r="A59" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C59" s="22"/>
-      <c r="D59" s="20" t="str">
+      <c r="C59" s="21" t="s">
+        <v>5553</v>
+      </c>
+      <c r="D59" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `PaintingFinishing`,</v>
+        <v>MOB_PAINTING_FINISHING AS `PaintingFinishing`,</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>205</v>
@@ -18445,13 +18581,15 @@
       <c r="A60" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B60" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="22"/>
-      <c r="D60" s="20" t="str">
+      <c r="C60" s="21" t="s">
+        <v>5554</v>
+      </c>
+      <c r="D60" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Coating`,</v>
+        <v>MOB_COATING AS `Coating`,</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>5504</v>
@@ -18467,13 +18605,15 @@
       <c r="A61" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="19" t="s">
+      <c r="B61" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="20" t="str">
+      <c r="C61" s="21" t="s">
+        <v>5555</v>
+      </c>
+      <c r="D61" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Type`,</v>
+        <v>MOB_TYPE AS `Type`,</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>5502</v>
@@ -18489,13 +18629,15 @@
       <c r="A62" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B62" s="18" t="s">
         <v>5489</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="20" t="str">
+      <c r="C62" s="21" t="s">
+        <v>5556</v>
+      </c>
+      <c r="D62" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `MaterialTableTop`,</v>
+        <v>MOB_MATERIAL_TABLE_TOP AS `MaterialTableTop`,</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>5501</v>
@@ -18511,13 +18653,15 @@
       <c r="A63" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C63" s="22"/>
-      <c r="D63" s="20" t="str">
+      <c r="C63" s="21" t="s">
+        <v>5557</v>
+      </c>
+      <c r="D63" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `FormatGl`,</v>
+        <v>MOB_FORMAT_GI AS `FormatGl`,</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>5500</v>
@@ -18533,13 +18677,15 @@
       <c r="A64" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B64" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="20" t="str">
+      <c r="C64" s="21" t="s">
+        <v>5558</v>
+      </c>
+      <c r="D64" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `Decorative`,</v>
+        <v>MOB_DECORATIVE AS `Decorative`,</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>5499</v>
@@ -18555,13 +18701,15 @@
       <c r="A65" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="B65" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C65" s="22"/>
-      <c r="D65" s="20" t="str">
+      <c r="C65" s="21" t="s">
+        <v>5559</v>
+      </c>
+      <c r="D65" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `TypeOfFootGl`,</v>
+        <v>MOB_TYPE_OF_FOOT_GI AS `TypeOfFootGl`,</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>5498</v>
@@ -18577,13 +18725,15 @@
       <c r="A66" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C66" s="22"/>
-      <c r="D66" s="20" t="str">
+      <c r="C66" s="21" t="s">
+        <v>5560</v>
+      </c>
+      <c r="D66" s="19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> AS `NumberOfDoors`,</v>
+        <v>MOB_NUMBER_OF_DOORS AS `NumberOfDoors`,</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>5497</v>
@@ -18597,13 +18747,15 @@
       <c r="A67" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B67" s="19" t="s">
+      <c r="B67" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C67" s="22"/>
-      <c r="D67" s="20" t="str">
-        <f t="shared" ref="D67:D73" si="2">CONCATENATE(C67, " AS `", B67, "`,")</f>
-        <v xml:space="preserve"> AS `NumberOfDrawers`,</v>
+      <c r="C67" s="21" t="s">
+        <v>5561</v>
+      </c>
+      <c r="D67" s="19" t="str">
+        <f t="shared" ref="D67:D73" si="3">CONCATENATE(C67, " AS `", B67, "`,")</f>
+        <v>MOB_NUMBER_OF_DRAWERS AS `NumberOfDrawers`,</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>5496</v>
@@ -18617,13 +18769,15 @@
       <c r="A68" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C68" s="22"/>
-      <c r="D68" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> AS `NumberOfShelves`,</v>
+      <c r="C68" s="21" t="s">
+        <v>5562</v>
+      </c>
+      <c r="D68" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>MOB_NUMBER_OF_SHELVES AS `NumberOfShelves`,</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>5495</v>
@@ -18637,13 +18791,15 @@
       <c r="A69" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B69" s="19" t="s">
+      <c r="B69" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="22"/>
-      <c r="D69" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> AS `LampNumber`,</v>
+      <c r="C69" s="21" t="s">
+        <v>5563</v>
+      </c>
+      <c r="D69" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>MOB_LAMP_NUMBER AS `LampNumber`,</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>5494</v>
@@ -18657,13 +18813,15 @@
       <c r="A70" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B70" s="19" t="s">
+      <c r="B70" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="22"/>
-      <c r="D70" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> AS `GlobalCapacity`,</v>
+      <c r="C70" s="21" t="s">
+        <v>5564</v>
+      </c>
+      <c r="D70" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>MOB_GLOBAL_CAPACITY AS `GlobalCapacity`,</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>5493</v>
@@ -18677,13 +18835,15 @@
       <c r="A71" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="19" t="s">
+      <c r="B71" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> AS `SocketType`,</v>
+      <c r="C71" s="21" t="s">
+        <v>5565</v>
+      </c>
+      <c r="D71" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>MOB_SOCKET_TYPE AS `SocketType`,</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>5492</v>
@@ -18697,13 +18857,15 @@
       <c r="A72" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B72" s="19" t="s">
+      <c r="B72" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> AS `VoltageHw`,</v>
+      <c r="C72" s="21" t="s">
+        <v>5566</v>
+      </c>
+      <c r="D72" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>MOB_VOLTAGE_HW AS `VoltageHw`,</v>
       </c>
       <c r="E72" s="17" t="s">
         <v>5491</v>
@@ -18717,13 +18879,15 @@
       <c r="A73" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B73" s="19" t="s">
+      <c r="B73" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> AS `AssemblyRequired`,</v>
+      <c r="C73" s="21" t="s">
+        <v>5567</v>
+      </c>
+      <c r="D73" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v>MOB_ASSEMBLY_REQUIRED AS `AssemblyRequired`,</v>
       </c>
       <c r="E73" s="17" t="s">
         <v>5490</v>

</xml_diff>

<commit_message>
Adicionados os campos da Mobly conforme exigências
</commit_message>
<xml_diff>
--- a/base/Template_Mobly.xlsx
+++ b/base/Template_Mobly.xlsx
@@ -1497,9 +1497,6 @@
     <t>ROUND(PRO_VALOR,2)</t>
   </si>
   <si>
-    <t>ROUND(PRO_PROMOCAO,2)</t>
-  </si>
-  <si>
     <t>PRO_PROMO_INI</t>
   </si>
   <si>
@@ -1515,9 +1512,6 @@
     <t>(SELECT CON_UF_LOJA FROM config LIMIT 0,1)</t>
   </si>
   <si>
-    <t>PRO_DESCRICAO</t>
-  </si>
-  <si>
     <t>MOB_COLOR</t>
   </si>
   <si>
@@ -1789,6 +1783,12 @@
   </si>
   <si>
     <t>49 peças</t>
+  </si>
+  <si>
+    <t>IF( $ePromo, ROUND(PRO_PROMOCAO,2), "")</t>
+  </si>
+  <si>
+    <t>$getDesc</t>
   </si>
 </sst>
 </file>
@@ -2318,7 +2318,7 @@
         <v>477</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>1</v>
@@ -2728,7 +2728,7 @@
         <v>43</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D19" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2752,7 +2752,7 @@
         <v>44</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D20" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2776,7 +2776,7 @@
         <v>48</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D21" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2800,7 +2800,7 @@
         <v>49</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D22" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2846,11 +2846,11 @@
         <v>56</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>490</v>
+        <v>586</v>
       </c>
       <c r="D24" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>ROUND(PRO_PROMOCAO,2) AS `SalePrice`,</v>
+        <v>IF( $ePromo, ROUND(PRO_PROMOCAO,2), "") AS `SalePrice`,</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>57</v>
@@ -2868,7 +2868,7 @@
         <v>59</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D25" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2890,7 +2890,7 @@
         <v>61</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D26" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3101,7 +3101,7 @@
         <v>75</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D36" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3125,7 +3125,7 @@
         <v>77</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D37" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3147,7 +3147,7 @@
         <v>78</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D38" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3212,7 +3212,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D41" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3234,7 +3234,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D42" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3256,11 +3256,11 @@
         <v>85</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>496</v>
+        <v>587</v>
       </c>
       <c r="D43" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>PRO_DESCRICAO AS `Description`,</v>
+        <v>$getDesc AS `Description`,</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>91</v>
@@ -3423,7 +3423,7 @@
         <v>99</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D51" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3445,7 +3445,7 @@
         <v>102</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D52" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3467,7 +3467,7 @@
         <v>103</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D53" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3489,7 +3489,7 @@
         <v>104</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D54" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3511,7 +3511,7 @@
         <v>105</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D55" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3533,7 +3533,7 @@
         <v>106</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D56" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3555,7 +3555,7 @@
         <v>444</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D57" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3579,7 +3579,7 @@
         <v>445</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D58" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3603,7 +3603,7 @@
         <v>107</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D59" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3627,7 +3627,7 @@
         <v>108</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D60" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3651,7 +3651,7 @@
         <v>109</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D61" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3675,7 +3675,7 @@
         <v>446</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D62" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3699,7 +3699,7 @@
         <v>110</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D63" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3723,7 +3723,7 @@
         <v>111</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D64" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3747,7 +3747,7 @@
         <v>112</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D65" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3771,7 +3771,7 @@
         <v>113</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D66" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3793,7 +3793,7 @@
         <v>114</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D67" s="11" t="str">
         <f t="shared" ref="D67:D73" si="3">CONCATENATE(C67, " AS `", B67, "`,")</f>
@@ -3815,7 +3815,7 @@
         <v>115</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D68" s="11" t="str">
         <f t="shared" si="3"/>
@@ -3837,7 +3837,7 @@
         <v>116</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D69" s="11" t="str">
         <f t="shared" si="3"/>
@@ -3859,7 +3859,7 @@
         <v>117</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D70" s="11" t="str">
         <f t="shared" si="3"/>
@@ -3881,7 +3881,7 @@
         <v>118</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D71" s="11" t="str">
         <f t="shared" si="3"/>
@@ -3903,7 +3903,7 @@
         <v>119</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D72" s="11" t="str">
         <f t="shared" si="3"/>
@@ -3925,7 +3925,7 @@
         <v>120</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D73" s="11" t="str">
         <f t="shared" si="3"/>
@@ -3965,148 +3965,148 @@
   <sheetData>
     <row r="1" spans="1:48" s="17" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>508</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>510</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="F1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>514</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>515</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>516</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>517</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>518</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="W1" s="15" t="s">
+        <v>520</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="Y1" s="15" t="s">
+        <v>521</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AA1" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AC1" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AE1" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AG1" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AI1" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AK1" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AM1" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AO1" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="AP1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AQ1" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="AR1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AS1" s="15" t="s">
         <v>511</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>512</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>514</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>515</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>516</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>517</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>518</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>519</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>520</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>521</v>
-      </c>
-      <c r="V1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="W1" s="15" t="s">
-        <v>522</v>
-      </c>
-      <c r="X1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="Y1" s="15" t="s">
-        <v>523</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AA1" s="15" t="s">
-        <v>497</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AC1" s="15" t="s">
-        <v>498</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AE1" s="15" t="s">
-        <v>499</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AG1" s="15" t="s">
-        <v>524</v>
-      </c>
-      <c r="AH1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>506</v>
-      </c>
-      <c r="AJ1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AK1" s="15" t="s">
-        <v>504</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AM1" s="15" t="s">
-        <v>500</v>
-      </c>
-      <c r="AN1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AO1" s="15" t="s">
-        <v>503</v>
-      </c>
-      <c r="AP1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AQ1" s="15" t="s">
+      <c r="AT1" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="AU1" s="15" t="s">
         <v>505</v>
       </c>
-      <c r="AR1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AS1" s="15" t="s">
-        <v>513</v>
-      </c>
-      <c r="AT1" s="16" t="s">
-        <v>494</v>
-      </c>
-      <c r="AU1" s="15" t="s">
-        <v>507</v>
-      </c>
       <c r="AV1" s="16" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2" spans="1:48" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4230,14 +4230,14 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_ASSEMBLY_REQUIRED','Sim, porém a montagem é simples e não sugerimos contratação de profissional');</v>
       </c>
       <c r="AI2" s="18" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="AJ2" s="18" t="str">
         <f>CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AI$1,"','",AI2,"');")</f>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_FOR_MATTRESS_TYPE','Berço (Convencional)');</v>
       </c>
       <c r="AK2" s="18" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AL2" s="18" t="str">
         <f>CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AK$1,"','",AK2,"');")</f>
@@ -4251,14 +4251,14 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Acrílico');</v>
       </c>
       <c r="AO2" s="18" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="AP2" s="18" t="str">
         <f t="shared" ref="AP2:AR17" si="0">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AO$1,"','",AO2,"');")</f>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_DIMENSIONS','de 180 a 220 cm');</v>
       </c>
       <c r="AQ2" s="18" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="AR2" s="18" t="str">
         <f t="shared" si="0"/>
@@ -4272,7 +4272,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Acrílico');</v>
       </c>
       <c r="AU2" s="18" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="AV2" s="18" t="str">
         <f t="shared" si="1"/>
@@ -4400,14 +4400,14 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_ASSEMBLY_REQUIRED','Não');</v>
       </c>
       <c r="AI3" s="18" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="AJ3" s="18" t="str">
         <f t="shared" ref="AJ3:AJ12" si="17">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AI$1,"','",AI3,"');")</f>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_FOR_MATTRESS_TYPE','Casal(128)');</v>
       </c>
       <c r="AK3" s="18" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="AL3" s="18" t="str">
         <f t="shared" ref="AL3:AL8" si="18">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AK$1,"','",AK3,"');")</f>
@@ -4421,14 +4421,14 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Algodão');</v>
       </c>
       <c r="AO3" s="18" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="AP3" s="18" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_DIMENSIONS','abaixo de 180 cm');</v>
       </c>
       <c r="AQ3" s="18" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="AR3" s="18" t="str">
         <f t="shared" si="0"/>
@@ -4442,7 +4442,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Algodão');</v>
       </c>
       <c r="AU3" s="18" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="AV3" s="18" t="str">
         <f t="shared" ref="AV3" si="20">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU3,"');")</f>
@@ -4560,14 +4560,14 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_ASSEMBLY_REQUIRED','Sim, sugerimos a contratação do nosso serviço de montagem (para os CEPs em que o serviço está disponível) ou de algum profissional experiente de sua preferência');</v>
       </c>
       <c r="AI4" s="18" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="AJ4" s="18" t="str">
         <f t="shared" si="17"/>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_FOR_MATTRESS_TYPE','Casal (138)');</v>
       </c>
       <c r="AK4" s="18" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="AL4" s="18" t="str">
         <f t="shared" si="18"/>
@@ -4581,14 +4581,14 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Alumínio');</v>
       </c>
       <c r="AO4" s="18" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="AP4" s="18" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_DIMENSIONS','100 x 150 cm');</v>
       </c>
       <c r="AQ4" s="18" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="AR4" s="18" t="str">
         <f t="shared" si="0"/>
@@ -4602,7 +4602,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Alumínio');</v>
       </c>
       <c r="AU4" s="18" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AV4" s="18" t="str">
         <f t="shared" ref="AV4" si="21">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU4,"');")</f>
@@ -4709,14 +4709,14 @@
       </c>
       <c r="AG5" s="18"/>
       <c r="AI5" s="18" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="AJ5" s="18" t="str">
         <f t="shared" si="17"/>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_FOR_MATTRESS_TYPE','King(198)');</v>
       </c>
       <c r="AK5" s="18" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="AL5" s="18" t="str">
         <f t="shared" si="18"/>
@@ -4730,14 +4730,14 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Antiaderente');</v>
       </c>
       <c r="AO5" s="18" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="AP5" s="18" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_DIMENSIONS','150 x 200 cm');</v>
       </c>
       <c r="AQ5" s="18" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="AR5" s="18" t="str">
         <f t="shared" si="0"/>
@@ -4751,7 +4751,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Antiaderente');</v>
       </c>
       <c r="AU5" s="18" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="AV5" s="18" t="str">
         <f t="shared" ref="AV5" si="22">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU5,"');")</f>
@@ -4853,14 +4853,14 @@
       </c>
       <c r="AG6" s="18"/>
       <c r="AI6" s="18" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="AJ6" s="18" t="str">
         <f t="shared" si="17"/>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_FOR_MATTRESS_TYPE','Queen(158)');</v>
       </c>
       <c r="AK6" s="18" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="AL6" s="18" t="str">
         <f t="shared" si="18"/>
@@ -4874,7 +4874,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Argila');</v>
       </c>
       <c r="AO6" s="18" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="AP6" s="18" t="str">
         <f t="shared" si="0"/>
@@ -4888,7 +4888,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Argila');</v>
       </c>
       <c r="AU6" s="18" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="AV6" s="18" t="str">
         <f t="shared" ref="AV6" si="23">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU6,"');")</f>
@@ -4985,14 +4985,14 @@
       </c>
       <c r="AG7" s="18"/>
       <c r="AI7" s="18" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="AJ7" s="18" t="str">
         <f t="shared" si="17"/>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_FOR_MATTRESS_TYPE','Solteiro(78)');</v>
       </c>
       <c r="AK7" s="18" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AL7" s="18" t="str">
         <f t="shared" si="18"/>
@@ -5006,7 +5006,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Aço');</v>
       </c>
       <c r="AO7" s="18" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="AP7" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5020,7 +5020,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Aço');</v>
       </c>
       <c r="AU7" s="18" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="AV7" s="18" t="str">
         <f t="shared" ref="AV7" si="24">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU7,"');")</f>
@@ -5117,14 +5117,14 @@
       </c>
       <c r="AG8" s="18"/>
       <c r="AI8" s="18" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AJ8" s="18" t="str">
         <f t="shared" si="17"/>
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_FOR_MATTRESS_TYPE','Solteiro(88)');</v>
       </c>
       <c r="AK8" s="18" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="AL8" s="18" t="str">
         <f t="shared" si="18"/>
@@ -5138,7 +5138,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Bambú');</v>
       </c>
       <c r="AO8" s="18" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="AP8" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5152,7 +5152,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Bambú');</v>
       </c>
       <c r="AU8" s="18" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="AV8" s="18" t="str">
         <f t="shared" ref="AV8" si="25">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU8,"');")</f>
@@ -5249,7 +5249,7 @@
       </c>
       <c r="AG9" s="18"/>
       <c r="AI9" s="18" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="AJ9" s="18" t="str">
         <f t="shared" si="17"/>
@@ -5263,7 +5263,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Borracha');</v>
       </c>
       <c r="AO9" s="18" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="AP9" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5277,7 +5277,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Borracha');</v>
       </c>
       <c r="AU9" s="18" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="AV9" s="18" t="str">
         <f t="shared" ref="AV9" si="26">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU9,"');")</f>
@@ -5374,7 +5374,7 @@
       </c>
       <c r="AG10" s="18"/>
       <c r="AI10" s="18" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="AJ10" s="18" t="str">
         <f t="shared" si="17"/>
@@ -5388,7 +5388,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Carbono');</v>
       </c>
       <c r="AO10" s="18" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="AP10" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5402,7 +5402,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Carbono');</v>
       </c>
       <c r="AU10" s="18" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="AV10" s="18" t="str">
         <f t="shared" ref="AV10" si="27">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU10,"');")</f>
@@ -5499,7 +5499,7 @@
       </c>
       <c r="AG11" s="18"/>
       <c r="AI11" s="18" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="AJ11" s="18" t="str">
         <f t="shared" si="17"/>
@@ -5513,7 +5513,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Carvão');</v>
       </c>
       <c r="AO11" s="18" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="AP11" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5527,7 +5527,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Carvão');</v>
       </c>
       <c r="AU11" s="18" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="AV11" s="18" t="str">
         <f t="shared" ref="AV11" si="28">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU11,"');")</f>
@@ -5614,7 +5614,7 @@
       </c>
       <c r="AG12" s="18"/>
       <c r="AI12" s="18" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="AJ12" s="18" t="str">
         <f t="shared" si="17"/>
@@ -5628,7 +5628,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Cerâmica');</v>
       </c>
       <c r="AO12" s="18" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="AP12" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5642,7 +5642,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Cerâmica');</v>
       </c>
       <c r="AU12" s="18" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="AV12" s="18" t="str">
         <f t="shared" ref="AV12" si="29">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU12,"');")</f>
@@ -5736,7 +5736,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Cetim');</v>
       </c>
       <c r="AO13" s="18" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="AP13" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5750,7 +5750,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Cetim');</v>
       </c>
       <c r="AU13" s="18" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="AV13" s="18" t="str">
         <f t="shared" ref="AV13" si="30">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU13,"');")</f>
@@ -5839,7 +5839,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Chenille');</v>
       </c>
       <c r="AO14" s="18" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="AP14" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5853,7 +5853,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Chenille');</v>
       </c>
       <c r="AU14" s="18" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="AV14" s="18" t="str">
         <f t="shared" ref="AV14" si="31">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU14,"');")</f>
@@ -5937,7 +5937,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Cobre');</v>
       </c>
       <c r="AO15" s="18" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="AP15" s="18" t="str">
         <f t="shared" si="0"/>
@@ -5951,7 +5951,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Cobre');</v>
       </c>
       <c r="AU15" s="18" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="AV15" s="18" t="str">
         <f t="shared" ref="AV15" si="32">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU15,"');")</f>
@@ -6030,7 +6030,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Couro Ecológico');</v>
       </c>
       <c r="AO16" s="18" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="AP16" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6044,7 +6044,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Couro Ecológico');</v>
       </c>
       <c r="AU16" s="18" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="AV16" s="18" t="str">
         <f t="shared" ref="AV16" si="33">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU16,"');")</f>
@@ -6123,7 +6123,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_FAMILY','Couro Natural');</v>
       </c>
       <c r="AO17" s="18" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="AP17" s="18" t="str">
         <f t="shared" si="0"/>
@@ -6137,7 +6137,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Couro Natural');</v>
       </c>
       <c r="AU17" s="18" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="AV17" s="18" t="str">
         <f t="shared" ref="AV17" si="34">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU17,"');")</f>
@@ -6218,7 +6218,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Couro Sintético');</v>
       </c>
       <c r="AU18" s="18" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="AV18" s="18" t="str">
         <f t="shared" ref="AV18" si="35">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU18,"');")</f>
@@ -6299,7 +6299,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Cristal');</v>
       </c>
       <c r="AU19" s="18" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="AV19" s="18" t="str">
         <f t="shared" ref="AV19" si="36">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU19,"');")</f>
@@ -6375,7 +6375,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Cromado');</v>
       </c>
       <c r="AU20" s="18" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="AV20" s="18" t="str">
         <f t="shared" ref="AV20" si="37">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU20,"');")</f>
@@ -6451,7 +6451,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Diamantado');</v>
       </c>
       <c r="AU21" s="18" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="AV21" s="18" t="str">
         <f t="shared" ref="AV21" si="38">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU21,"');")</f>
@@ -6527,7 +6527,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','DS33');</v>
       </c>
       <c r="AU22" s="18" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="AV22" s="18" t="str">
         <f t="shared" ref="AV22" si="39">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU22,"');")</f>
@@ -6603,7 +6603,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Elastano');</v>
       </c>
       <c r="AU23" s="18" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="AV23" s="18" t="str">
         <f t="shared" ref="AV23" si="40">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU23,"');")</f>
@@ -6679,7 +6679,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Espuma');</v>
       </c>
       <c r="AU24" s="18" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="AV24" s="18" t="str">
         <f t="shared" ref="AV24" si="41">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU24,"');")</f>
@@ -6755,7 +6755,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','Eucalipto');</v>
       </c>
       <c r="AU25" s="18" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="AV25" s="18" t="str">
         <f t="shared" ref="AV25" si="42">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU25,"');")</f>
@@ -6831,7 +6831,7 @@
         <v>INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('MOB_MATERIAL_TABLE_TOP','EVA');</v>
       </c>
       <c r="AU26" s="18" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="AV26" s="18" t="str">
         <f t="shared" ref="AV26" si="43">CONCATENATE("INSERT INTO mobly_list (MOB_FIELD, MOB_OPTION) VALUES ('",AU$1,"','",AU26,"');")</f>

</xml_diff>